<commit_message>
set up unscaled results
</commit_message>
<xml_diff>
--- a/revision/complete_comparison_fcps/job_status.xlsx
+++ b/revision/complete_comparison_fcps/job_status.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hollywiberg/git/Optimal_Clustering_Trees/revision/complete_comparison_fcps/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96DF2C47-B039-614E-B7CD-C7F11BA9E2BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2CDB086-879E-6F41-9E35-FD460B464F3D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5960" yWindow="460" windowWidth="18320" windowHeight="16040" xr2:uid="{473B9B2E-87E6-CE4B-90BD-76DCCF73FCE0}"/>
+    <workbookView xWindow="11040" yWindow="460" windowWidth="18320" windowHeight="16040" xr2:uid="{473B9B2E-87E6-CE4B-90BD-76DCCF73FCE0}"/>
   </bookViews>
   <sheets>
     <sheet name="seeds1345" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="20">
   <si>
     <t>data</t>
   </si>
@@ -88,13 +88,7 @@
     <t>s</t>
   </si>
   <si>
-    <t>Notes</t>
-  </si>
-  <si>
     <t>In progress</t>
-  </si>
-  <si>
-    <t>IAI (node1114)</t>
   </si>
   <si>
     <t>Status</t>
@@ -104,7 +98,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -119,13 +113,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -140,15 +147,36 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -481,8 +509,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E88EA017-3DFA-BF41-850D-CD946131C6B6}">
   <dimension ref="A1:H91"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="43" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="A62" zoomScale="125" zoomScaleNormal="43" workbookViewId="0">
+      <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -507,11 +535,8 @@
       <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
-        <v>18</v>
-      </c>
       <c r="H1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -528,7 +553,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="2">
-        <v>111.32850000000001</v>
+        <v>85.529163999999994</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -548,7 +573,7 @@
         <v>1</v>
       </c>
       <c r="E3" s="2">
-        <v>117.4431</v>
+        <v>158.958552</v>
       </c>
       <c r="F3">
         <v>2</v>
@@ -568,7 +593,7 @@
         <v>1</v>
       </c>
       <c r="E4" s="2">
-        <v>3309.5410000000002</v>
+        <v>3063.0959250000001</v>
       </c>
       <c r="F4">
         <v>3</v>
@@ -588,7 +613,7 @@
         <v>1</v>
       </c>
       <c r="E5" s="2">
-        <v>12.025869999999999</v>
+        <v>7.4865409999999999</v>
       </c>
       <c r="F5">
         <v>4</v>
@@ -608,7 +633,7 @@
         <v>1</v>
       </c>
       <c r="E6" s="2">
-        <v>22.28378</v>
+        <v>21.954151</v>
       </c>
       <c r="F6">
         <v>5</v>
@@ -628,7 +653,7 @@
         <v>1</v>
       </c>
       <c r="E7" s="2">
-        <v>105.7089</v>
+        <v>78.541743999999994</v>
       </c>
       <c r="F7">
         <v>6</v>
@@ -648,7 +673,7 @@
         <v>1</v>
       </c>
       <c r="E8" s="2">
-        <v>19.247319999999998</v>
+        <v>17.591602000000002</v>
       </c>
       <c r="F8">
         <v>7</v>
@@ -668,7 +693,7 @@
         <v>1</v>
       </c>
       <c r="E9" s="2">
-        <v>26.65971</v>
+        <v>21.215278999999999</v>
       </c>
       <c r="F9">
         <v>8</v>
@@ -688,7 +713,7 @@
         <v>1</v>
       </c>
       <c r="E10" s="2">
-        <v>74.27816</v>
+        <v>70.721097999999998</v>
       </c>
       <c r="F10">
         <v>9</v>
@@ -708,7 +733,7 @@
         <v>1</v>
       </c>
       <c r="E11" s="2">
-        <v>390.59910000000002</v>
+        <v>190.086455</v>
       </c>
       <c r="F11">
         <v>10</v>
@@ -728,7 +753,7 @@
         <v>1</v>
       </c>
       <c r="E12" s="2">
-        <v>611.52509999999995</v>
+        <v>731.52028399999995</v>
       </c>
       <c r="F12">
         <v>11</v>
@@ -747,11 +772,14 @@
       <c r="D13">
         <v>1</v>
       </c>
-      <c r="E13" s="2">
-        <v>39289.910000000003</v>
+      <c r="E13" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="F13">
         <v>12</v>
+      </c>
+      <c r="G13" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
@@ -768,7 +796,7 @@
         <v>1</v>
       </c>
       <c r="E14" s="2">
-        <v>10.75067</v>
+        <v>9.7955959999999997</v>
       </c>
       <c r="F14">
         <v>13</v>
@@ -788,7 +816,7 @@
         <v>1</v>
       </c>
       <c r="E15" s="2">
-        <v>73.236689999999996</v>
+        <v>77.512294999999995</v>
       </c>
       <c r="F15">
         <v>14</v>
@@ -808,7 +836,7 @@
         <v>1</v>
       </c>
       <c r="E16" s="2">
-        <v>173.64439999999999</v>
+        <v>134.43170000000001</v>
       </c>
       <c r="F16">
         <v>15</v>
@@ -828,7 +856,7 @@
         <v>1</v>
       </c>
       <c r="E17" s="2">
-        <v>22.404579999999999</v>
+        <v>20.125874</v>
       </c>
       <c r="F17">
         <v>16</v>
@@ -848,7 +876,7 @@
         <v>1</v>
       </c>
       <c r="E18" s="2">
-        <v>416.69900000000001</v>
+        <v>200.85098099999999</v>
       </c>
       <c r="F18">
         <v>17</v>
@@ -868,7 +896,7 @@
         <v>1</v>
       </c>
       <c r="E19" s="2">
-        <v>227.5711</v>
+        <v>200.95983699999999</v>
       </c>
       <c r="F19">
         <v>18</v>
@@ -885,10 +913,10 @@
         <v>6</v>
       </c>
       <c r="D20">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E20" s="2">
-        <v>92.312290000000004</v>
+        <v>90.239795999999998</v>
       </c>
       <c r="F20">
         <v>19</v>
@@ -905,10 +933,10 @@
         <v>6</v>
       </c>
       <c r="D21">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E21" s="2">
-        <v>119.6253</v>
+        <v>145.48911699999999</v>
       </c>
       <c r="F21">
         <v>20</v>
@@ -925,10 +953,10 @@
         <v>6</v>
       </c>
       <c r="D22">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E22" s="2">
-        <v>3145.511</v>
+        <v>3288.082997</v>
       </c>
       <c r="F22">
         <v>21</v>
@@ -945,10 +973,10 @@
         <v>6</v>
       </c>
       <c r="D23">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E23" s="2">
-        <v>12.260389999999999</v>
+        <v>8.5863589999999999</v>
       </c>
       <c r="F23">
         <v>22</v>
@@ -965,11 +993,9 @@
         <v>6</v>
       </c>
       <c r="D24">
-        <v>3</v>
-      </c>
-      <c r="E24" s="2">
-        <v>20.095009999999998</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="E24" s="2"/>
       <c r="F24">
         <v>23</v>
       </c>
@@ -985,10 +1011,10 @@
         <v>6</v>
       </c>
       <c r="D25">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E25" s="2">
-        <v>110.59050000000001</v>
+        <v>88.998548</v>
       </c>
       <c r="F25">
         <v>24</v>
@@ -1005,10 +1031,10 @@
         <v>6</v>
       </c>
       <c r="D26">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E26" s="2">
-        <v>19.058959999999999</v>
+        <v>17.443207000000001</v>
       </c>
       <c r="F26">
         <v>25</v>
@@ -1025,10 +1051,10 @@
         <v>6</v>
       </c>
       <c r="D27">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E27" s="2">
-        <v>23.16939</v>
+        <v>21.145911999999999</v>
       </c>
       <c r="F27">
         <v>26</v>
@@ -1045,10 +1071,10 @@
         <v>6</v>
       </c>
       <c r="D28">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E28" s="2">
-        <v>81.587190000000007</v>
+        <v>69.785764999999998</v>
       </c>
       <c r="F28">
         <v>27</v>
@@ -1065,10 +1091,10 @@
         <v>16</v>
       </c>
       <c r="D29">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E29" s="2">
-        <v>325.77179999999998</v>
+        <v>169.77055200000001</v>
       </c>
       <c r="F29">
         <v>28</v>
@@ -1085,10 +1111,10 @@
         <v>16</v>
       </c>
       <c r="D30">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E30" s="2">
-        <v>474.4178</v>
+        <v>1153.120443</v>
       </c>
       <c r="F30">
         <v>29</v>
@@ -1105,7 +1131,7 @@
         <v>16</v>
       </c>
       <c r="D31">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E31" t="s">
         <v>7</v>
@@ -1114,7 +1140,7 @@
         <v>30</v>
       </c>
       <c r="G31" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
@@ -1128,10 +1154,10 @@
         <v>16</v>
       </c>
       <c r="D32">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E32" s="2">
-        <v>10.34215</v>
+        <v>9.7266600000000007</v>
       </c>
       <c r="F32">
         <v>31</v>
@@ -1148,10 +1174,10 @@
         <v>16</v>
       </c>
       <c r="D33">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E33" s="2">
-        <v>69.486459999999994</v>
+        <v>96.099193</v>
       </c>
       <c r="F33">
         <v>32</v>
@@ -1169,11 +1195,9 @@
         <v>16</v>
       </c>
       <c r="D34">
-        <v>3</v>
-      </c>
-      <c r="E34" s="2">
-        <v>153.2527</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="E34" s="2"/>
       <c r="F34">
         <v>33</v>
       </c>
@@ -1189,10 +1213,10 @@
         <v>16</v>
       </c>
       <c r="D35">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E35" s="2">
-        <v>22.36383</v>
+        <v>20.582295999999999</v>
       </c>
       <c r="F35">
         <v>34</v>
@@ -1209,10 +1233,10 @@
         <v>16</v>
       </c>
       <c r="D36">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E36" s="2">
-        <v>442.28789999999998</v>
+        <v>302.61093299999999</v>
       </c>
       <c r="F36">
         <v>35</v>
@@ -1229,10 +1253,10 @@
         <v>16</v>
       </c>
       <c r="D37">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E37" s="2">
-        <v>266.16950000000003</v>
+        <v>208.21483900000001</v>
       </c>
       <c r="F37">
         <v>36</v>
@@ -1249,10 +1273,10 @@
         <v>6</v>
       </c>
       <c r="D38">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E38" s="2">
-        <v>89.616169999999997</v>
+        <v>120.843847</v>
       </c>
       <c r="F38">
         <v>37</v>
@@ -1269,10 +1293,10 @@
         <v>6</v>
       </c>
       <c r="D39">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E39" s="2">
-        <v>125.6722</v>
+        <v>157.997601</v>
       </c>
       <c r="F39">
         <v>38</v>
@@ -1289,13 +1313,16 @@
         <v>6</v>
       </c>
       <c r="D40">
-        <v>4</v>
-      </c>
-      <c r="E40" s="2">
-        <v>3124.201</v>
+        <v>3</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="F40">
         <v>39</v>
+      </c>
+      <c r="G40" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
@@ -1309,16 +1336,13 @@
         <v>6</v>
       </c>
       <c r="D41">
-        <v>4</v>
-      </c>
-      <c r="E41" t="s">
-        <v>7</v>
+        <v>3</v>
+      </c>
+      <c r="E41">
+        <v>8.4943259999999992</v>
       </c>
       <c r="F41">
         <v>40</v>
-      </c>
-      <c r="G41" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
@@ -1332,10 +1356,10 @@
         <v>6</v>
       </c>
       <c r="D42">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E42" s="2">
-        <v>22.591940000000001</v>
+        <v>20.819109000000001</v>
       </c>
       <c r="F42">
         <v>41</v>
@@ -1353,10 +1377,10 @@
         <v>6</v>
       </c>
       <c r="D43">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E43" s="2">
-        <v>119.9406</v>
+        <v>81.823260000000005</v>
       </c>
       <c r="F43">
         <v>42</v>
@@ -1373,10 +1397,10 @@
         <v>6</v>
       </c>
       <c r="D44">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E44" s="2">
-        <v>18.603069999999999</v>
+        <v>17.672439000000001</v>
       </c>
       <c r="F44">
         <v>43</v>
@@ -1393,10 +1417,10 @@
         <v>6</v>
       </c>
       <c r="D45">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E45" s="2">
-        <v>22.51802</v>
+        <v>21.354068000000002</v>
       </c>
       <c r="F45">
         <v>44</v>
@@ -1414,10 +1438,10 @@
         <v>6</v>
       </c>
       <c r="D46">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E46" s="2">
-        <v>80.212919999999997</v>
+        <v>70.856386000000001</v>
       </c>
       <c r="F46">
         <v>45</v>
@@ -1434,10 +1458,10 @@
         <v>16</v>
       </c>
       <c r="D47">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E47" s="2">
-        <v>265.81610000000001</v>
+        <v>221.930992</v>
       </c>
       <c r="F47">
         <v>46</v>
@@ -1454,17 +1478,15 @@
         <v>16</v>
       </c>
       <c r="D48">
-        <v>4</v>
-      </c>
-      <c r="E48" t="s">
-        <v>7</v>
+        <v>3</v>
+      </c>
+      <c r="E48">
+        <v>624.68474600000002</v>
       </c>
       <c r="F48">
         <v>47</v>
       </c>
-      <c r="G48" s="1" t="s">
-        <v>20</v>
-      </c>
+      <c r="G48" s="1"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49">
@@ -1477,7 +1499,7 @@
         <v>16</v>
       </c>
       <c r="D49">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E49" t="s">
         <v>7</v>
@@ -1486,7 +1508,7 @@
         <v>48</v>
       </c>
       <c r="G49" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
@@ -1500,10 +1522,10 @@
         <v>16</v>
       </c>
       <c r="D50">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E50" s="2">
-        <v>9.8037949999999991</v>
+        <v>9.4707319999999999</v>
       </c>
       <c r="F50">
         <v>49</v>
@@ -1521,13 +1543,16 @@
         <v>16</v>
       </c>
       <c r="D51">
-        <v>4</v>
-      </c>
-      <c r="E51" s="2">
-        <v>75.106920000000002</v>
+        <v>3</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="F51">
         <v>50</v>
+      </c>
+      <c r="G51" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
@@ -1541,10 +1566,10 @@
         <v>16</v>
       </c>
       <c r="D52">
-        <v>4</v>
-      </c>
-      <c r="E52" t="s">
-        <v>7</v>
+        <v>3</v>
+      </c>
+      <c r="E52">
+        <v>142.805543</v>
       </c>
       <c r="F52">
         <v>51</v>
@@ -1561,10 +1586,10 @@
         <v>16</v>
       </c>
       <c r="D53">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E53" s="2">
-        <v>21.83248</v>
+        <v>20.780878000000001</v>
       </c>
       <c r="F53">
         <v>52</v>
@@ -1581,10 +1606,10 @@
         <v>16</v>
       </c>
       <c r="D54">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E54" s="2">
-        <v>388.6968</v>
+        <v>864.46672000000001</v>
       </c>
       <c r="F54">
         <v>53</v>
@@ -1601,10 +1626,10 @@
         <v>16</v>
       </c>
       <c r="D55">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E55" s="2">
-        <v>245.01910000000001</v>
+        <v>228.21425500000001</v>
       </c>
       <c r="F55">
         <v>54</v>
@@ -1621,10 +1646,10 @@
         <v>6</v>
       </c>
       <c r="D56">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E56" s="2">
-        <v>106.7071</v>
+        <v>142.41031000000001</v>
       </c>
       <c r="F56">
         <v>55</v>
@@ -1641,10 +1666,10 @@
         <v>6</v>
       </c>
       <c r="D57">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E57" s="2">
-        <v>116.0368</v>
+        <v>153.260255</v>
       </c>
       <c r="F57">
         <v>56</v>
@@ -1661,10 +1686,10 @@
         <v>6</v>
       </c>
       <c r="D58">
-        <v>5</v>
-      </c>
-      <c r="E58" t="s">
-        <v>7</v>
+        <v>4</v>
+      </c>
+      <c r="E58">
+        <v>3150.6725029999998</v>
       </c>
       <c r="F58">
         <v>57</v>
@@ -1681,10 +1706,10 @@
         <v>6</v>
       </c>
       <c r="D59">
-        <v>5</v>
-      </c>
-      <c r="E59" s="2">
-        <v>12.519959999999999</v>
+        <v>4</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="F59">
         <v>58</v>
@@ -1701,10 +1726,10 @@
         <v>6</v>
       </c>
       <c r="D60">
-        <v>5</v>
-      </c>
-      <c r="E60" t="s">
-        <v>7</v>
+        <v>4</v>
+      </c>
+      <c r="E60">
+        <v>21.006360999999998</v>
       </c>
       <c r="F60">
         <v>59</v>
@@ -1721,10 +1746,10 @@
         <v>6</v>
       </c>
       <c r="D61">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E61" s="2">
-        <v>111.2662</v>
+        <v>82.061054999999996</v>
       </c>
       <c r="F61">
         <v>60</v>
@@ -1741,10 +1766,10 @@
         <v>6</v>
       </c>
       <c r="D62">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E62" s="2">
-        <v>18.725180000000002</v>
+        <v>17.533550000000002</v>
       </c>
       <c r="F62">
         <v>61</v>
@@ -1761,10 +1786,10 @@
         <v>6</v>
       </c>
       <c r="D63">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E63" s="2">
-        <v>22.467120000000001</v>
+        <v>21.321145999999999</v>
       </c>
       <c r="F63">
         <v>62</v>
@@ -1781,16 +1806,16 @@
         <v>6</v>
       </c>
       <c r="D64">
-        <v>5</v>
-      </c>
-      <c r="E64" s="2">
-        <v>75.776079999999993</v>
+        <v>4</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="F64">
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>64</v>
       </c>
@@ -1801,16 +1826,16 @@
         <v>16</v>
       </c>
       <c r="D65">
-        <v>5</v>
-      </c>
-      <c r="E65" t="s">
-        <v>7</v>
+        <v>4</v>
+      </c>
+      <c r="E65">
+        <v>217.03029599999999</v>
       </c>
       <c r="F65">
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>65</v>
       </c>
@@ -1821,16 +1846,16 @@
         <v>16</v>
       </c>
       <c r="D66">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E66" s="2">
-        <v>509.58839999999998</v>
+        <v>744.63148699999999</v>
       </c>
       <c r="F66">
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>66</v>
       </c>
@@ -1841,7 +1866,7 @@
         <v>16</v>
       </c>
       <c r="D67">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E67" t="s">
         <v>7</v>
@@ -1849,8 +1874,11 @@
       <c r="F67">
         <v>66</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G67" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>67</v>
       </c>
@@ -1861,16 +1889,16 @@
         <v>16</v>
       </c>
       <c r="D68">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E68" s="2">
-        <v>10.262499999999999</v>
+        <v>9.6125969999999992</v>
       </c>
       <c r="F68">
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>68</v>
       </c>
@@ -1881,16 +1909,16 @@
         <v>16</v>
       </c>
       <c r="D69">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E69" s="2">
-        <v>65.293840000000003</v>
+        <v>67.329054999999997</v>
       </c>
       <c r="F69">
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>69</v>
       </c>
@@ -1901,16 +1929,16 @@
         <v>16</v>
       </c>
       <c r="D70">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E70" s="2">
-        <v>140.7928</v>
+        <v>138.983225</v>
       </c>
       <c r="F70">
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>70</v>
       </c>
@@ -1921,16 +1949,16 @@
         <v>16</v>
       </c>
       <c r="D71">
-        <v>5</v>
-      </c>
-      <c r="E71" s="2">
-        <v>21.891970000000001</v>
+        <v>4</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="F71">
         <v>70</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>71</v>
       </c>
@@ -1941,16 +1969,16 @@
         <v>16</v>
       </c>
       <c r="D72">
-        <v>5</v>
-      </c>
-      <c r="E72" t="s">
-        <v>7</v>
+        <v>4</v>
+      </c>
+      <c r="E72">
+        <v>923.94941400000005</v>
       </c>
       <c r="F72">
         <v>71</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>72</v>
       </c>
@@ -1961,16 +1989,16 @@
         <v>16</v>
       </c>
       <c r="D73">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E73" s="2">
-        <v>295.35509999999999</v>
+        <v>202.475101</v>
       </c>
       <c r="F73">
         <v>72</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>73</v>
       </c>
@@ -1981,16 +2009,16 @@
         <v>6</v>
       </c>
       <c r="D74">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E74" s="2">
-        <v>92.001350000000002</v>
+        <v>82.610196000000002</v>
       </c>
       <c r="F74">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>74</v>
       </c>
@@ -2001,16 +2029,16 @@
         <v>6</v>
       </c>
       <c r="D75">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E75" s="2">
-        <v>115.6446</v>
+        <v>155.277637</v>
       </c>
       <c r="F75">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>75</v>
       </c>
@@ -2021,16 +2049,16 @@
         <v>6</v>
       </c>
       <c r="D76">
-        <v>2</v>
-      </c>
-      <c r="E76" s="2">
-        <v>3391.6889999999999</v>
+        <v>5</v>
+      </c>
+      <c r="E76" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="F76">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>76</v>
       </c>
@@ -2041,16 +2069,16 @@
         <v>6</v>
       </c>
       <c r="D77">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E77" s="2">
-        <v>12.227460000000001</v>
+        <v>8.6564309999999995</v>
       </c>
       <c r="F77">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>77</v>
       </c>
@@ -2061,16 +2089,16 @@
         <v>6</v>
       </c>
       <c r="D78">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E78" s="2">
-        <v>0.34084710000000001</v>
+        <v>19.703854</v>
       </c>
       <c r="F78">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>78</v>
       </c>
@@ -2081,16 +2109,16 @@
         <v>6</v>
       </c>
       <c r="D79">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E79" s="2">
-        <v>96.205500000000001</v>
+        <v>71.544793999999996</v>
       </c>
       <c r="F79">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>79</v>
       </c>
@@ -2101,16 +2129,16 @@
         <v>6</v>
       </c>
       <c r="D80">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E80" s="2">
-        <v>19.300180000000001</v>
+        <v>17.770005999999999</v>
       </c>
       <c r="F80">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>80</v>
       </c>
@@ -2121,16 +2149,16 @@
         <v>6</v>
       </c>
       <c r="D81">
-        <v>2</v>
-      </c>
-      <c r="E81" s="2">
-        <v>22.28341</v>
+        <v>5</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="F81">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>81</v>
       </c>
@@ -2141,16 +2169,16 @@
         <v>6</v>
       </c>
       <c r="D82">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E82" s="2">
-        <v>78.359970000000004</v>
+        <v>69.902325000000005</v>
       </c>
       <c r="F82">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>82</v>
       </c>
@@ -2161,16 +2189,16 @@
         <v>16</v>
       </c>
       <c r="D83">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E83" s="2">
-        <v>392.90460000000002</v>
+        <v>199.678404</v>
       </c>
       <c r="F83">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>83</v>
       </c>
@@ -2181,16 +2209,16 @@
         <v>16</v>
       </c>
       <c r="D84">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E84" s="2">
-        <v>643.45740000000001</v>
+        <v>659.85692400000005</v>
       </c>
       <c r="F84">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>84</v>
       </c>
@@ -2201,16 +2229,19 @@
         <v>16</v>
       </c>
       <c r="D85">
-        <v>2</v>
-      </c>
-      <c r="E85" s="2">
-        <v>32661.93</v>
+        <v>5</v>
+      </c>
+      <c r="E85" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="F85">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+        <v>84</v>
+      </c>
+      <c r="G85" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>85</v>
       </c>
@@ -2221,16 +2252,16 @@
         <v>16</v>
       </c>
       <c r="D86">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E86" s="2">
-        <v>10.57638</v>
+        <v>9.5769280000000006</v>
       </c>
       <c r="F86">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>86</v>
       </c>
@@ -2241,16 +2272,16 @@
         <v>16</v>
       </c>
       <c r="D87">
-        <v>2</v>
-      </c>
-      <c r="E87" s="2">
-        <v>71.101290000000006</v>
+        <v>5</v>
+      </c>
+      <c r="E87" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="F87">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>87</v>
       </c>
@@ -2261,16 +2292,16 @@
         <v>16</v>
       </c>
       <c r="D88">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E88" s="2">
-        <v>165.3595</v>
+        <v>139.76759899999999</v>
       </c>
       <c r="F88">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>88</v>
       </c>
@@ -2281,16 +2312,16 @@
         <v>16</v>
       </c>
       <c r="D89">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E89" s="2">
-        <v>22.07151</v>
+        <v>20.315452000000001</v>
       </c>
       <c r="F89">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>89</v>
       </c>
@@ -2301,16 +2332,16 @@
         <v>16</v>
       </c>
       <c r="D90">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E90" s="2">
-        <v>407.81079999999997</v>
+        <v>111.901866</v>
       </c>
       <c r="F90">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>90</v>
       </c>
@@ -2321,19 +2352,34 @@
         <v>16</v>
       </c>
       <c r="D91">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E91" s="2">
-        <v>212.4736</v>
+        <v>216.627599</v>
       </c>
       <c r="F91">
-        <v>18</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:F91">
-    <cfRule type="expression" dxfId="1" priority="1">
+  <conditionalFormatting sqref="B2:F91 G13 G59 G51 G40">
+    <cfRule type="expression" dxfId="3" priority="4">
       <formula>$E2="NA"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G31">
+    <cfRule type="expression" dxfId="2" priority="3">
+      <formula>$E31="NA"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G49">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>$E49="NA"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G67">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>$E67="NA"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>